<commit_message>
Updated progress report for week 2
</commit_message>
<xml_diff>
--- a/Progress Report - Group A.xlsx
+++ b/Progress Report - Group A.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Loyalist College\Semester 1\AISC1006 - Step Presentation (Step 1) 01\week 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Loyalist College\STEP\Project\Telecom-Churn-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{94A4FB75-0AC7-9043-A3E7-E37375CA1980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E79FE25E-4FD0-E24E-BAD0-EF7AE3A4AE20}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD17DA0-F4EC-4F11-B989-29E5F0AD2108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
   <si>
     <t>Team Members</t>
   </si>
@@ -149,7 +149,40 @@
     <t>On Week 1, Each member came up with 2 project ideas and presented to the group to decide on the final project idea.</t>
   </si>
   <si>
-    <t>On Week 2, Each member was introduced to the dataset,GitHub, Kaggle and Jupyter notebook.</t>
+    <t>Attribute analysis(gender &amp; seniorCitizen)</t>
+  </si>
+  <si>
+    <t>Attribute analysis(Contract &amp; PaperlessBilling)</t>
+  </si>
+  <si>
+    <t>Attribute analysis(DeviceProtection &amp; TechSupport)</t>
+  </si>
+  <si>
+    <t>Attribute introduction,analysis and presentation preparation</t>
+  </si>
+  <si>
+    <t>Presentation preparation &amp; attribute analysis(Partner,Dependents,tenure)</t>
+  </si>
+  <si>
+    <t>Dataset analysis and visualization(StreamingTV,StreamingMovies)</t>
+  </si>
+  <si>
+    <t>Presentation Preparation &amp; Dataset understanding(PhoneService,MultipleLines,InternetService)</t>
+  </si>
+  <si>
+    <t>Attribute analysis(OnlineSecurity,OnlineBackup)</t>
+  </si>
+  <si>
+    <t>Week 4, Dataset was divided among each member and was introduced to the basics of Jupyter notebook, Pandas and matplotlib. Presentation was created by the team with everybody present, so that we could brainstorm and collaborate to get suggestions.</t>
+  </si>
+  <si>
+    <t>On Week 3, Each member was introduced to the dataset,GitHub, Kaggle and Jupyter notebook.</t>
+  </si>
+  <si>
+    <t>Dataset Discovery</t>
+  </si>
+  <si>
+    <t>On week 2, The project was decided on and the team was introduced to the dataset and its attributes as well as the introduction to kaggle.</t>
   </si>
 </sst>
 </file>
@@ -218,15 +251,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -509,20 +547,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C30" sqref="C29:C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.48046875" customWidth="1"/>
-    <col min="2" max="2" width="37.93359375" customWidth="1"/>
-    <col min="3" max="3" width="38.0703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="37.88671875" customWidth="1"/>
+    <col min="3" max="3" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="79.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -530,7 +570,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
@@ -538,12 +578,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -551,7 +591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -559,7 +599,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -567,7 +607,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -575,7 +615,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -583,7 +623,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -591,7 +631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -599,7 +639,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -607,8 +647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>28</v>
       </c>
@@ -621,8 +660,9 @@
       <c r="E16" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -630,10 +670,16 @@
         <v>34</v>
       </c>
       <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -641,10 +687,16 @@
         <v>34</v>
       </c>
       <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -652,10 +704,16 @@
         <v>34</v>
       </c>
       <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -663,10 +721,16 @@
         <v>34</v>
       </c>
       <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -674,10 +738,16 @@
         <v>34</v>
       </c>
       <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -685,10 +755,16 @@
         <v>34</v>
       </c>
       <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -696,10 +772,16 @@
         <v>34</v>
       </c>
       <c r="C23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -707,18 +789,30 @@
         <v>34</v>
       </c>
       <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="41.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="E24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>37</v>
+        <v>48</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Progress Report - Group A.xlsx
</commit_message>
<xml_diff>
--- a/Progress Report - Group A.xlsx
+++ b/Progress Report - Group A.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Loyalist College\STEP\Project\Telecom-Churn-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD17DA0-F4EC-4F11-B989-29E5F0AD2108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4C6051-07B2-4556-ADB8-84BB1FC1023F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
   <si>
     <t>Team Members</t>
   </si>
@@ -183,6 +183,15 @@
   </si>
   <si>
     <t>On week 2, The project was decided on and the team was introduced to the dataset and its attributes as well as the introduction to kaggle.</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Dataset analysis, Missing values identification</t>
+  </si>
+  <si>
+    <t>Week 5, Dataset analysis was continued while learning how to use different python libraries. Target variable imbalance was identified on the dataset.</t>
   </si>
 </sst>
 </file>
@@ -251,12 +260,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -547,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C30" sqref="C29:C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,9 +568,10 @@
     <col min="3" max="3" width="38.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="79.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -570,7 +579,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
@@ -578,12 +587,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -591,7 +600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -599,7 +608,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -607,7 +616,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -615,7 +624,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -623,7 +632,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -631,7 +640,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -639,7 +648,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -647,7 +656,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>28</v>
       </c>
@@ -660,9 +669,11 @@
       <c r="E16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -678,8 +689,11 @@
       <c r="E17" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -695,8 +709,11 @@
       <c r="E18" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -712,8 +729,11 @@
       <c r="E19" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -729,8 +749,11 @@
       <c r="E20" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -746,8 +769,11 @@
       <c r="E21" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -763,8 +789,11 @@
       <c r="E22" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -780,8 +809,11 @@
       <c r="E23" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -797,22 +829,28 @@
       <c r="E24" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
+      <c r="F24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="4" t="s">
         <v>45</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>